<commit_message>
Updates list of requirements
</commit_message>
<xml_diff>
--- a/Documents/Requirements/Requirements.xlsx
+++ b/Documents/Requirements/Requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Number</t>
   </si>
@@ -54,18 +54,12 @@
     <t>1.2.3</t>
   </si>
   <si>
-    <t>admins shall be able to remove sites</t>
-  </si>
-  <si>
     <t>Section 2</t>
   </si>
   <si>
     <t>User Functions</t>
   </si>
   <si>
-    <t>The user shall be able to identify start and end locations</t>
-  </si>
-  <si>
     <t>Section 3</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>The system shall provide help files for users and admins</t>
   </si>
   <si>
-    <t>The system shall calculate the shortest route between all chosen locations</t>
-  </si>
-  <si>
     <t>The system shall display the calculated route on Google Earth</t>
   </si>
   <si>
@@ -93,7 +84,31 @@
     <t>Platform</t>
   </si>
   <si>
-    <t>[Once decided, the host environment required]</t>
+    <t>User actions shall be performed in a graphical user interface</t>
+  </si>
+  <si>
+    <t>The system shall calculate the shortest route between all locations, starting at the chosen start waypoint and terminating at the chosen end waypoint</t>
+  </si>
+  <si>
+    <t>Admins shall be able to remove sites</t>
+  </si>
+  <si>
+    <t>The user shall be able to identify start and end "waypoints"</t>
+  </si>
+  <si>
+    <t>The system shall include all US national parks as waypoints</t>
+  </si>
+  <si>
+    <t>The system shall include Machu Picchu as a waypoint</t>
+  </si>
+  <si>
+    <t>The system shall calculate the final route distance</t>
+  </si>
+  <si>
+    <t>The system shall include a facts display for each waypoint</t>
+  </si>
+  <si>
+    <t>The GUI shall be blue and green</t>
   </si>
 </sst>
 </file>
@@ -146,7 +161,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -154,6 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -496,27 +511,27 @@
     <col min="2" max="2" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
@@ -524,7 +539,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -532,7 +547,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
@@ -540,19 +555,19 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -560,15 +575,15 @@
         <v>2.1</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -576,7 +591,7 @@
         <v>3.1</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -584,7 +599,7 @@
         <v>3.2</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -592,7 +607,7 @@
         <v>3.3</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -600,7 +615,7 @@
         <v>3.4</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -608,23 +623,63 @@
         <v>3.5</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="3" customFormat="1">
-      <c r="A18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>3.6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>3.7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
+        <v>3.8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>3.9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
+      <c r="B23" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>4.2</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>